<commit_message>
fix errors in data, visualize clean data
</commit_message>
<xml_diff>
--- a/code/data/raw/pDeltaT.xlsx
+++ b/code/data/raw/pDeltaT.xlsx
@@ -219,8 +219,8 @@
   </sheetPr>
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2025,10 +2025,10 @@
         <v>13</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>114.165</v>
@@ -2057,10 +2057,10 @@
         <v>13</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>30.2974</v>
@@ -2121,10 +2121,10 @@
         <v>13</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>0.504457</v>
@@ -2153,10 +2153,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>0.0556598</v>
@@ -2185,10 +2185,10 @@
         <v>13</v>
       </c>
       <c r="B62" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>209.372</v>
@@ -2217,10 +2217,10 @@
         <v>13</v>
       </c>
       <c r="B63" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C63" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>46.2721</v>
@@ -2249,10 +2249,10 @@
         <v>13</v>
       </c>
       <c r="B64" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C64" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>12.4501</v>
@@ -2281,10 +2281,10 @@
         <v>13</v>
       </c>
       <c r="B65" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C65" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>0.495052</v>
@@ -2313,10 +2313,10 @@
         <v>13</v>
       </c>
       <c r="B66" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="C66" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>150</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>0.0536142</v>
@@ -2345,10 +2345,10 @@
         <v>13</v>
       </c>
       <c r="B67" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>277.121</v>
@@ -2377,10 +2377,10 @@
         <v>13</v>
       </c>
       <c r="B68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C68" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C68" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>49.5886</v>
@@ -2409,10 +2409,10 @@
         <v>13</v>
       </c>
       <c r="B69" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C69" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>12.5016</v>
@@ -2441,10 +2441,10 @@
         <v>13</v>
       </c>
       <c r="B70" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C70" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>0.493066</v>
@@ -2473,10 +2473,10 @@
         <v>13</v>
       </c>
       <c r="B71" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="C71" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C71" s="1" t="n">
-        <v>150</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>0.0547306</v>
@@ -2505,10 +2505,10 @@
         <v>13</v>
       </c>
       <c r="B72" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>298.047</v>
@@ -2537,10 +2537,10 @@
         <v>13</v>
       </c>
       <c r="B73" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C73" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>50.0504</v>
@@ -2569,10 +2569,10 @@
         <v>13</v>
       </c>
       <c r="B74" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C74" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>12.5572</v>
@@ -2601,10 +2601,10 @@
         <v>13</v>
       </c>
       <c r="B75" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C75" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>0.496833</v>
@@ -2633,10 +2633,10 @@
         <v>13</v>
       </c>
       <c r="B76" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="C76" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>150</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>0.0545242</v>
@@ -2665,10 +2665,10 @@
         <v>14</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>100.158</v>
@@ -2697,10 +2697,10 @@
         <v>14</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>29.099</v>
@@ -2761,10 +2761,10 @@
         <v>14</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>0.526</v>
@@ -2793,10 +2793,10 @@
         <v>14</v>
       </c>
       <c r="B81" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C81" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>203.652</v>
@@ -2825,10 +2825,10 @@
         <v>14</v>
       </c>
       <c r="B82" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C82" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>47.052</v>
@@ -2857,10 +2857,10 @@
         <v>14</v>
       </c>
       <c r="B83" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C83" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>12.861</v>
@@ -2889,10 +2889,10 @@
         <v>14</v>
       </c>
       <c r="B84" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C84" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="C84" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>0.053</v>
@@ -2921,10 +2921,10 @@
         <v>14</v>
       </c>
       <c r="B85" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C85" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>277.775</v>
@@ -2953,10 +2953,10 @@
         <v>14</v>
       </c>
       <c r="B86" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C86" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>51.444</v>
@@ -2985,10 +2985,10 @@
         <v>14</v>
       </c>
       <c r="B87" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C87" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C87" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>13.198</v>
@@ -3017,10 +3017,10 @@
         <v>14</v>
       </c>
       <c r="B88" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C88" s="1" t="n">
         <v>60</v>
-      </c>
-      <c r="C88" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>0.533</v>
@@ -3049,10 +3049,10 @@
         <v>14</v>
       </c>
       <c r="B89" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C89" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C89" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>304.309</v>
@@ -3081,10 +3081,10 @@
         <v>14</v>
       </c>
       <c r="B90" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C90" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>52.427</v>
@@ -3113,10 +3113,10 @@
         <v>14</v>
       </c>
       <c r="B91" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C91" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C91" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>13.267</v>
@@ -3145,10 +3145,10 @@
         <v>14</v>
       </c>
       <c r="B92" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C92" s="1" t="n">
         <v>90</v>
-      </c>
-      <c r="C92" s="1" t="n">
-        <v>50</v>
       </c>
       <c r="D92" s="1" t="n">
         <v>0.533</v>

</xml_diff>